<commit_message>
added in links and administrative contacts
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D90736-9F51-B14D-891C-76D7A013E2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A95A2D-1F9C-CB4D-B207-560D360484EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -409,13 +409,117 @@
   </si>
   <si>
     <t xml:space="preserve">Mulitple locations </t>
+  </si>
+  <si>
+    <t>https://vcwnorthern.com/eye-programs/</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/1597/VIEW-Vehicles-for-Change</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/3302/Local-Bus</t>
+  </si>
+  <si>
+    <t>http://transportation.dmas.virginia.gov/</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/1699/On-Demand-Transportation</t>
+  </si>
+  <si>
+    <t>https://www.coverva.org/en/famis</t>
+  </si>
+  <si>
+    <t>https://www.coverva.org/en/adults-19-64-years-old</t>
+  </si>
+  <si>
+    <t>https://www.loudoun.gov/4111/Continuum-of-Care-Programs-Partnerships</t>
+  </si>
+  <si>
+    <t>https://vcwnorthern.com/about/</t>
+  </si>
+  <si>
+    <t>https://www.vccs.edu/wp-content/uploads/2020/04/FINANCIAL-AID-PROGRAMS-revised-100719.pdf</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Teens-Young-Adults/412-Youth-Zone.aspx</t>
+  </si>
+  <si>
+    <t>downloads a pdf
+https://www.alleghenycounty.us/WorkArea/linkit.aspx?LinkIdentifier=id&amp;ItemID=2147493264</t>
+  </si>
+  <si>
+    <t>https://www.auberle.org/employment-institute</t>
+  </si>
+  <si>
+    <t>https://familylinks.org/get-help/housing/DOCS</t>
+  </si>
+  <si>
+    <t>https://www.transitionalservices.org/programs/psychiatric-disabilities/transition-age-youth-tay</t>
+  </si>
+  <si>
+    <t>https://actionhousing.org/our-services/myplace-youth-program/</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Northern Virginia Community College</t>
+  </si>
+  <si>
+    <t>Viriginia Department of Social Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun County Public Schools </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Virginia Family Service </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun County </t>
+  </si>
+  <si>
+    <t>Virginia Department of Medical Assistance Services</t>
+  </si>
+  <si>
+    <t>Department of Family Services</t>
+  </si>
+  <si>
+    <t>Local Department of Social Services</t>
+  </si>
+  <si>
+    <t>US Department of Housing and Urban Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SkillSource </t>
+  </si>
+  <si>
+    <t>Department of Human Services</t>
+  </si>
+  <si>
+    <t>Abby Wolensky
+Deputy Director of the Employment Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FamilyLInk </t>
+  </si>
+  <si>
+    <t>Community Care Behavioral Health Organization</t>
+  </si>
+  <si>
+    <t>Sharon Langford</t>
+  </si>
+  <si>
+    <t>Rachael Tichacek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun County Department of Transit and Commuter Services </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +544,43 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color rgb="FF5E514E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF1D1D26"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -461,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -472,6 +613,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,22 +939,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="45.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="39.1640625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="61.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="68.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="27" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="3" customWidth="1"/>
     <col min="12" max="12" width="25" style="3" customWidth="1"/>
     <col min="13" max="13" width="64.6640625" style="3" customWidth="1"/>
     <col min="14" max="14" width="24.1640625" style="3" customWidth="1"/>
@@ -889,7 +1041,9 @@
         <v>-77.115129999999994</v>
       </c>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="N2" s="1" t="s">
         <v>118</v>
       </c>
@@ -929,7 +1083,9 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="N3" s="1" t="s">
         <v>119</v>
       </c>
@@ -968,7 +1124,9 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="N4" s="1" t="s">
         <v>120</v>
       </c>
@@ -1009,7 +1167,9 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N5" s="1" t="s">
         <v>121</v>
       </c>
@@ -1050,7 +1210,9 @@
         <v>-77.400989999999993</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N6" s="1" t="s">
         <v>121</v>
       </c>
@@ -1091,7 +1253,9 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N7" s="1" t="s">
         <v>121</v>
       </c>
@@ -1131,8 +1295,12 @@
       <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N8" s="1" t="s">
         <v>121</v>
       </c>
@@ -1173,12 +1341,14 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N9" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>9</v>
@@ -1212,10 +1382,14 @@
         <v>-77.539617175199197</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="M10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="85" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A10+1</f>
         <v>10</v>
@@ -1251,7 +1425,9 @@
         <v>-77.539617175199197</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="M11" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="N11" s="1" t="s">
         <v>122</v>
       </c>
@@ -1292,8 +1468,12 @@
         <v>-77.231870559863694</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1353,7 +1533,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1388,9 +1568,15 @@
       <c r="K15" s="1">
         <v>-77.555404002188297</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1427,11 +1613,17 @@
       <c r="K16" s="1">
         <v>-77.340073015724201</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="L16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1464,9 +1656,15 @@
         <v>123</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1499,9 +1697,15 @@
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1534,11 +1738,17 @@
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="L19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1569,9 +1779,15 @@
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1604,9 +1820,15 @@
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1639,11 +1861,17 @@
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="L22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1674,11 +1902,15 @@
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="N23" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="126" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1714,10 +1946,14 @@
         <v>-80.001456359819201</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" ht="63" x14ac:dyDescent="0.2">
+      <c r="M24" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="147" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1753,10 +1989,14 @@
         <v>-80.001021344478104</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" ht="105" x14ac:dyDescent="0.2">
+      <c r="M25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="106" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1792,10 +2032,14 @@
         <v>-79.832162824794494</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="M26" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="127" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1831,10 +2075,14 @@
         <v>-79.994721902148598</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="M27" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="127" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1868,10 +2116,14 @@
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="M28" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="85" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1907,10 +2159,14 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+      <c r="M29" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="85" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1946,10 +2202,14 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" ht="147" x14ac:dyDescent="0.2">
+      <c r="M30" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="148" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1983,8 +2243,12 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+      <c r="M31" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A32" s="1">

</xml_diff>

<commit_message>
added towns and some more latitude/longitude
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A95A2D-1F9C-CB4D-B207-560D360484EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D18D95-E795-584C-B26D-DDC4DA8FECA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -403,9 +403,6 @@
   </si>
   <si>
     <t>https://vcwnorthern.com/youth-programs/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple locations </t>
   </si>
   <si>
     <t xml:space="preserve">Mulitple locations </t>
@@ -513,6 +510,30 @@
   </si>
   <si>
     <t xml:space="preserve">Loudoun County Department of Transit and Commuter Services </t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Ashburn</t>
+  </si>
+  <si>
+    <t>Leesburg</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>McKeesport</t>
+  </si>
+  <si>
+    <t>Pittsburgh and McKeesport</t>
   </si>
 </sst>
 </file>
@@ -939,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1040,9 +1061,11 @@
       <c r="K2" s="1">
         <v>-77.115129999999994</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="M2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>118</v>
@@ -1082,9 +1105,11 @@
       <c r="K3" s="1">
         <v>-77.437179999999998</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>119</v>
@@ -1123,9 +1148,11 @@
       <c r="K4" s="1">
         <v>-77.437179999999998</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="M4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>120</v>
@@ -1166,9 +1193,11 @@
       <c r="K5" s="1">
         <v>-77.520380000000003</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="M5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>121</v>
@@ -1209,9 +1238,11 @@
       <c r="K6" s="1">
         <v>-77.400989999999993</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="M6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>121</v>
@@ -1252,9 +1283,11 @@
       <c r="K7" s="1">
         <v>-77.520380000000003</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="M7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>121</v>
@@ -1296,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>121</v>
@@ -1340,9 +1373,11 @@
       <c r="K9" s="1">
         <v>-77.520380000000003</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="M9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>121</v>
@@ -1381,12 +1416,14 @@
       <c r="K10" s="1">
         <v>-77.539617175199197</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="M10" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="85" x14ac:dyDescent="0.25">
@@ -1424,9 +1461,11 @@
       <c r="K11" s="1">
         <v>-77.539617175199197</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="M11" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>122</v>
@@ -1467,12 +1506,14 @@
       <c r="K12" s="1">
         <v>-77.231870559863694</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="M12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -1569,13 +1610,13 @@
         <v>-77.555404002188297</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -1614,13 +1655,13 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="N16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="84" x14ac:dyDescent="0.2">
@@ -1652,18 +1693,20 @@
       <c r="I17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K17" s="1"/>
+      <c r="J17" s="1">
+        <v>39.114571664302197</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-77.5405475733521</v>
+      </c>
       <c r="L17" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -1695,16 +1738,20 @@
       <c r="I18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
       <c r="L18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="63" x14ac:dyDescent="0.2">
@@ -1736,19 +1783,23 @@
       <c r="I19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
       <c r="L19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1777,19 +1828,23 @@
       <c r="I20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
       <c r="L20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="84" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1818,16 +1873,20 @@
       <c r="I21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
       <c r="L21" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="84" x14ac:dyDescent="0.2">
@@ -1859,13 +1918,17 @@
       <c r="I22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
       <c r="L22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>119</v>
@@ -1900,14 +1963,18 @@
       <c r="I23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
       <c r="L23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="126" x14ac:dyDescent="0.2">
@@ -1945,12 +2012,14 @@
       <c r="K24" s="1">
         <v>-80.001456359819201</v>
       </c>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M24" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="147" x14ac:dyDescent="0.2">
@@ -1988,12 +2057,14 @@
       <c r="K25" s="1">
         <v>-80.001021344478104</v>
       </c>
-      <c r="L25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M25" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="106" x14ac:dyDescent="0.25">
@@ -2031,12 +2102,14 @@
       <c r="K26" s="1">
         <v>-79.832162824794494</v>
       </c>
-      <c r="L26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="M26" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="127" x14ac:dyDescent="0.25">
@@ -2074,12 +2147,14 @@
       <c r="K27" s="1">
         <v>-79.994721902148598</v>
       </c>
-      <c r="L27" s="1"/>
+      <c r="L27" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M27" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="127" x14ac:dyDescent="0.25">
@@ -2112,15 +2187,17 @@
         <v>109</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="M28" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="85" x14ac:dyDescent="0.25">
@@ -2158,12 +2235,14 @@
       <c r="K29" s="1">
         <v>-79.835243102149704</v>
       </c>
-      <c r="L29" s="1"/>
+      <c r="L29" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M29" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="85" x14ac:dyDescent="0.25">
@@ -2201,12 +2280,14 @@
       <c r="K30" s="1">
         <v>-79.835243102149704</v>
       </c>
-      <c r="L30" s="1"/>
+      <c r="L30" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M30" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="148" x14ac:dyDescent="0.25">
@@ -2242,12 +2323,14 @@
       <c r="K31" s="1">
         <v>-79.835243102149704</v>
       </c>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="M31" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added information on transportation and insurance
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D18D95-E795-584C-B26D-DDC4DA8FECA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0994693B-7C4E-654A-A8C1-9E8D82012ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -534,13 +534,83 @@
   </si>
   <si>
     <t>Pittsburgh and McKeesport</t>
+  </si>
+  <si>
+    <t>Self Sufficiency Program</t>
+  </si>
+  <si>
+    <t>Live in a household whose total income is no more than 200% of the federal Income Poverty Guidelines</t>
+  </si>
+  <si>
+    <t>This program has services that are for the TAY if they would have roadblocks keeping them from getting ahead or earn less than what they need to live. The services would help the TAY figure out their strengths and weakness, create a plan to reach their goals, and connect to those resources to help them achieve their goals</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Self-Sufficiency-Case-Management,-Training,-and-Job-Placement.aspx</t>
+  </si>
+  <si>
+    <t>Behavioral Health Transportation</t>
+  </si>
+  <si>
+    <t>Be receiving behavioral health services from a BHTP-participating, Department of Human services (DHS)- contracted provider. Live at least one-half mile from an eligible destination AND 
+Start attending at least three eligible trips per week as stated in service plan. An eligible trip is any trip you need to take as part of your personal recovery journey: dinner with a friend or family; a trip to the grocery store; AA or NA, Anything that’s in your plan can count as an eligible trip.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This program helps citizens that need transportation due to a behavioral health condition. It is for any service that will help them be able to function as an individual while receiving care. </t>
+  </si>
+  <si>
+    <t>Medicial Assistance Transportation Program</t>
+  </si>
+  <si>
+    <t>This program provides free public transportation (bus, subway and incline) ahead-of-time ticket, reimbursement for your use of public transportation or a private car, and free door-to-door service, when medically necessary, via shared-ride or ride-hailing service.</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Health Insurance Marketplace</t>
+  </si>
+  <si>
+    <t>Alleghany Activates</t>
+  </si>
+  <si>
+    <t>Behavioral Health Insurance (mental health, alcohol, drug, or other addiction services)</t>
+  </si>
+  <si>
+    <t>Community Behavioral Health Organization (community Care) is the behavioral health managed care organization for Allegheny County residents who receive Medical Assistance.</t>
+  </si>
+  <si>
+    <t>Mental Health Rx Pharmacy Benefit Program</t>
+  </si>
+  <si>
+    <t>Providing psychiatric prescription medications at no cost to eligible individuals. Eligibility is based on income.</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Transportation/Medical-Assistance-Transportation-Program.aspx</t>
+  </si>
+  <si>
+    <t>Medical Assistance (Medicaid) “MA”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides free health care coverage to low-income Pennsylvania residents. Residents should fit into one of the eligibility groups that are covered by the program and have income, and sometimes resources, which fall below the level set by the state for their category of MA eligibility.   </t>
+  </si>
+  <si>
+    <t>low-income Pennsylvania residents</t>
+  </si>
+  <si>
+    <t>https://www.compass.state.pa.us/compass.web/Public/CMPHome</t>
+  </si>
+  <si>
+    <t>healthcare.gov</t>
+  </si>
+  <si>
+    <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Health-Insurance.aspx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -602,6 +672,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -620,10 +711,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,8 +736,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="F33" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -969,11 +1084,11 @@
     <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="52.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="39.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="61.6640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="27" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.5" style="3" customWidth="1"/>
@@ -1160,7 +1275,7 @@
     </row>
     <row r="5" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A35" si="0">A4+1</f>
+        <f t="shared" ref="A5:A39" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2290,7 +2405,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="148" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="106" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2333,7 +2448,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="189" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2341,90 +2456,247 @@
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
+      <c r="N32" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="252" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="H33" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>172</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
+      <c r="N33" s="15"/>
+    </row>
+    <row r="34" spans="1:14" ht="231" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="N34" s="19" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="35" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="H35" s="14"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="N35" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="14"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f>A32+1</f>
+        <v>32</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" t="s">
+        <v>185</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="126" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" t="s">
+        <v>185</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L40" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N32" r:id="rId1" xr:uid="{60C613F1-CC52-7A4D-8822-A803097073DE}"/>
+    <hyperlink ref="N34" r:id="rId2" xr:uid="{A4D4722A-F053-934D-97DC-12F1F10D2CC7}"/>
+    <hyperlink ref="N36" r:id="rId3" xr:uid="{6B18FC7C-EE3D-6D44-B9DF-7F93B7653470}"/>
+    <hyperlink ref="N37:N38" r:id="rId4" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Health-Insurance.aspx" xr:uid="{A6720D7E-3399-D843-87D0-0CB86745C76A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filled in missing information
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24443645-384A-7447-8BB0-D7D47B25C458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E27BA0-9535-8A43-93E7-72ACAFE3CFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -1037,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2521,8 +2521,12 @@
       <c r="E35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2547,8 +2551,12 @@
       <c r="E36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2576,8 +2584,12 @@
       <c r="E37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
         <v>179</v>
@@ -2607,8 +2619,12 @@
       <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H38" s="8" t="s">
         <v>185</v>
       </c>
@@ -2640,8 +2656,12 @@
       <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H39" s="8" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
i'm not sure. i'm sorry
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E27BA0-9535-8A43-93E7-72ACAFE3CFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A8FC0-3677-2942-B844-6B7B22478259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
+    <workbookView xWindow="580" yWindow="5080" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1037,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added fairfax into spreadsheet
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/Qualitative_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A8FC0-3677-2942-B844-6B7B22478259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E369416-64D5-954C-9143-0B19F25A5BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="5080" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="227">
   <si>
     <t>ID</t>
   </si>
@@ -604,13 +604,141 @@
   </si>
   <si>
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Health-Insurance.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax </t>
+  </si>
+  <si>
+    <t>Second Story for Homeless Youth</t>
+  </si>
+  <si>
+    <t>Meet U.S. Department of Housing and Urban Development’s (HUD) definition of homelessness, meaning they are living in a homeless shelter, sleeping on the streets or another place not meant for human habitation, or fleeing domestic violence in Fairfax County, and be referred by a community provider</t>
+  </si>
+  <si>
+    <t>https://www.second-story.org/homeless-youth/</t>
+  </si>
+  <si>
+    <t>Long-term housing and support for youth aged 18-24 who are experiencing homelessness or living in an unsafe situation; Youth often come to us who have aged out of foster care, been kicked out of their parent or guardian’s home with insufficient resources, or have run away from an unsafe situation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunn Loring </t>
+  </si>
+  <si>
+    <t>LIFT One</t>
+  </si>
+  <si>
+    <t>LIFT TWO</t>
+  </si>
+  <si>
+    <t>Bridging Affordability</t>
+  </si>
+  <si>
+    <t>17-21</t>
+  </si>
+  <si>
+    <t>focuses on providing: subsidized apartments that provide stable housing to homeless youth, viable vocational/career skills-building &amp; training, life skills prep, support services (including: shelter, food, clothing, medical assistance, crisis intervention, counseling, referrals &amp; aftercare services)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need a referral </t>
+  </si>
+  <si>
+    <t>Receive housing, vocational and educational services, life skills training, therapeutic services (counseling, therapy and/or substance abuse education), and the development of a network of support services in the community; apartment-based Independent Living and Support Services to help foster care youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chantilly </t>
+  </si>
+  <si>
+    <t>https://mycri.org/services/youth-services/lift-program</t>
+  </si>
+  <si>
+    <t>https://www.nvfs.org/assistance/bridging-affordability/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referred by Fairfax County, working preference, earning 30% to 50% of area median income (AMI), living or working in Fairfax County, Not open referral </t>
+  </si>
+  <si>
+    <t>provides case management and supportive services like job training and financial education, depending on client needs, as well as rental assistance for up to 24 months</t>
+  </si>
+  <si>
+    <t>Oakton</t>
+  </si>
+  <si>
+    <t>Secondary Transition to Employment Program (STEP)</t>
+  </si>
+  <si>
+    <t>18-22</t>
+  </si>
+  <si>
+    <t>Receive instruction in applied academics, self-advocacy, and independent living skills</t>
+  </si>
+  <si>
+    <t>Falls Church</t>
+  </si>
+  <si>
+    <t>https://www.fcps.edu/academics/academic-overview/special-education-instruction/career-and-transition-services/step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax County Adult High School, Diploma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-21 or 22+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Springfield </t>
+  </si>
+  <si>
+    <t>https://fairfaxadulths.fcps.edu/about</t>
+  </si>
+  <si>
+    <t>helps prepare *Fairfax County residents  to take the GED test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax resident </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daytime: M-F (five days a week); five class periods lasting 75 minutes each and a 30 minute learning seminar; semester program
+Evening: Two 90 minute classes nightly M-W and/or T-Th; year-long classes
+Day program tuition is $80.00 per semester
+Evening program tuition is $160.00 per school year
+General Education students aged 18—19 do not pay tuition
+English Language Learners (ELLs) aged 18—21 do not pay tuition </t>
+  </si>
+  <si>
+    <t>Permanency and Life Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provides SAT prep, application fees, and dorm supplies, household items, moving fees and gift cards for gas, transportation, Department of Family Services </t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/familyservices/children-youth/permanency-life-skills</t>
+  </si>
+  <si>
+    <t>TOPS - Transportation Options, Programs &amp; Services</t>
+  </si>
+  <si>
+    <t>Must be a resident of Fairfax County or the City of Fairfax, plus meet one of the following criteria:
+50 years of age or older, with an annual income of $50,000 or less per household
+registered user of MetroAccess
+recipient of Supplemental Security Income (SSI) or Social Security Disability Insurance (SSDI)
+annual income that meets the 225% federal poverty levels by household size</t>
+  </si>
+  <si>
+    <t>Options:
+Taxicabs
+Rideshare services (Uber and Lyft)
+Public Transportation: bus and rail via SmarTrip card
+Capital BikeShare rentals; 
+Apply online or send in application</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/tops</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -669,6 +797,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -691,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -718,6 +859,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1035,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A48" sqref="A40:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1383,7 @@
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A39" si="0">A4+1</f>
+        <f t="shared" ref="A5:A53" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2676,8 +2822,453 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L40" s="1"/>
+    <row r="40" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="J40" s="2">
+        <v>38.906303508879397</v>
+      </c>
+      <c r="K40" s="2">
+        <v>-77.222641329237604</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J41" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="K41" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J42" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="K42" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J43" s="2">
+        <v>38.873610192974397</v>
+      </c>
+      <c r="K43" s="2">
+        <v>-77.3055466310296</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="J44" s="2">
+        <v>38.868590773014198</v>
+      </c>
+      <c r="K44" s="2">
+        <v>-77.224144877053305</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="147" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J45" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="K45" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J46" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="K46" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J47" s="2">
+        <v>38.8553917225858</v>
+      </c>
+      <c r="K47" s="2">
+        <v>-77.362718702194798</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J48" s="2">
+        <v>38.854251580169802</v>
+      </c>
+      <c r="K48" s="2">
+        <v>-77.356579302194902</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="E54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
trying to add in slider map of zip codes
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\Loudoun\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850779D0-0472-4B2A-B773-5526F4FC1401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E369416-64D5-954C-9143-0B19F25A5BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="227">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>On Demand Transportation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurances </t>
   </si>
   <si>
     <t xml:space="preserve">Funding &amp; Policy </t>
@@ -561,6 +564,9 @@
     <t>This program provides free public transportation (bus, subway and incline) ahead-of-time ticket, reimbursement for your use of public transportation or a private car, and free door-to-door service, when medically necessary, via shared-ride or ride-hailing service.</t>
   </si>
   <si>
+    <t>Insurance</t>
+  </si>
+  <si>
     <t>Health Insurance Marketplace</t>
   </si>
   <si>
@@ -600,17 +606,139 @@
     <t>https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Health-Insurance.aspx</t>
   </si>
   <si>
-    <t xml:space="preserve">Health </t>
-  </si>
-  <si>
-    <t>Health</t>
+    <t xml:space="preserve">Fairfax </t>
+  </si>
+  <si>
+    <t>Second Story for Homeless Youth</t>
+  </si>
+  <si>
+    <t>Meet U.S. Department of Housing and Urban Development’s (HUD) definition of homelessness, meaning they are living in a homeless shelter, sleeping on the streets or another place not meant for human habitation, or fleeing domestic violence in Fairfax County, and be referred by a community provider</t>
+  </si>
+  <si>
+    <t>https://www.second-story.org/homeless-youth/</t>
+  </si>
+  <si>
+    <t>Long-term housing and support for youth aged 18-24 who are experiencing homelessness or living in an unsafe situation; Youth often come to us who have aged out of foster care, been kicked out of their parent or guardian’s home with insufficient resources, or have run away from an unsafe situation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunn Loring </t>
+  </si>
+  <si>
+    <t>LIFT One</t>
+  </si>
+  <si>
+    <t>LIFT TWO</t>
+  </si>
+  <si>
+    <t>Bridging Affordability</t>
+  </si>
+  <si>
+    <t>17-21</t>
+  </si>
+  <si>
+    <t>focuses on providing: subsidized apartments that provide stable housing to homeless youth, viable vocational/career skills-building &amp; training, life skills prep, support services (including: shelter, food, clothing, medical assistance, crisis intervention, counseling, referrals &amp; aftercare services)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need a referral </t>
+  </si>
+  <si>
+    <t>Receive housing, vocational and educational services, life skills training, therapeutic services (counseling, therapy and/or substance abuse education), and the development of a network of support services in the community; apartment-based Independent Living and Support Services to help foster care youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chantilly </t>
+  </si>
+  <si>
+    <t>https://mycri.org/services/youth-services/lift-program</t>
+  </si>
+  <si>
+    <t>https://www.nvfs.org/assistance/bridging-affordability/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referred by Fairfax County, working preference, earning 30% to 50% of area median income (AMI), living or working in Fairfax County, Not open referral </t>
+  </si>
+  <si>
+    <t>provides case management and supportive services like job training and financial education, depending on client needs, as well as rental assistance for up to 24 months</t>
+  </si>
+  <si>
+    <t>Oakton</t>
+  </si>
+  <si>
+    <t>Secondary Transition to Employment Program (STEP)</t>
+  </si>
+  <si>
+    <t>18-22</t>
+  </si>
+  <si>
+    <t>Receive instruction in applied academics, self-advocacy, and independent living skills</t>
+  </si>
+  <si>
+    <t>Falls Church</t>
+  </si>
+  <si>
+    <t>https://www.fcps.edu/academics/academic-overview/special-education-instruction/career-and-transition-services/step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax County Adult High School, Diploma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-21 or 22+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Springfield </t>
+  </si>
+  <si>
+    <t>https://fairfaxadulths.fcps.edu/about</t>
+  </si>
+  <si>
+    <t>helps prepare *Fairfax County residents  to take the GED test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairfax resident </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daytime: M-F (five days a week); five class periods lasting 75 minutes each and a 30 minute learning seminar; semester program
+Evening: Two 90 minute classes nightly M-W and/or T-Th; year-long classes
+Day program tuition is $80.00 per semester
+Evening program tuition is $160.00 per school year
+General Education students aged 18—19 do not pay tuition
+English Language Learners (ELLs) aged 18—21 do not pay tuition </t>
+  </si>
+  <si>
+    <t>Permanency and Life Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provides SAT prep, application fees, and dorm supplies, household items, moving fees and gift cards for gas, transportation, Department of Family Services </t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/familyservices/children-youth/permanency-life-skills</t>
+  </si>
+  <si>
+    <t>TOPS - Transportation Options, Programs &amp; Services</t>
+  </si>
+  <si>
+    <t>Must be a resident of Fairfax County or the City of Fairfax, plus meet one of the following criteria:
+50 years of age or older, with an annual income of $50,000 or less per household
+registered user of MetroAccess
+recipient of Supplemental Security Income (SSI) or Social Security Disability Insurance (SSDI)
+annual income that meets the 225% federal poverty levels by household size</t>
+  </si>
+  <si>
+    <t>Options:
+Taxicabs
+Rideshare services (Uber and Lyft)
+Public Transportation: bus and rail via SmarTrip card
+Capital BikeShare rentals; 
+Apply online or send in application</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/tops</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -624,53 +752,10 @@
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="16"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="17"/>
-      <color rgb="FF5E514E"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF1D1D26"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -681,17 +766,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
+      <sz val="18"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="10"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -713,9 +830,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -723,40 +840,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1073,32 +1181,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A48" sqref="A40:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="20.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="52.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="61.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="27" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25" style="3" customWidth="1"/>
-    <col min="13" max="13" width="64.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.1640625" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="11.1640625" style="3"/>
+    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="125.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="119" style="2" customWidth="1"/>
+    <col min="10" max="10" width="27" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="40" style="2" customWidth="1"/>
+    <col min="13" max="13" width="64.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="114.1640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="102.5">
+    <row r="1" spans="1:14" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,34 +1223,34 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="81" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1159,16 +1267,16 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="J2" s="1">
         <v>38.840490000000003</v>
@@ -1177,16 +1285,16 @@
         <v>-77.115129999999994</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="61.5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1203,16 +1311,16 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1">
         <v>37.538339999999998</v>
@@ -1221,16 +1329,16 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="61.5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>3</v>
@@ -1248,14 +1356,14 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4" s="1">
         <v>37.538339999999998</v>
@@ -1264,18 +1372,18 @@
         <v>-77.437179999999998</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="41">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A39" si="0">A4+1</f>
+        <f t="shared" ref="A5:A53" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1291,16 +1399,16 @@
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="J5" s="1">
         <v>39.031359999999999</v>
@@ -1309,16 +1417,16 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="61.5">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1336,16 +1444,16 @@
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="J6" s="1">
         <v>39.015009999999997</v>
@@ -1354,16 +1462,16 @@
         <v>-77.400989999999993</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="41">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1381,13 +1489,13 @@
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>21</v>
@@ -1399,16 +1507,16 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="82">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1426,13 +1534,13 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
@@ -1444,16 +1552,16 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="41">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1471,13 +1579,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>19</v>
@@ -1489,16 +1597,16 @@
         <v>-77.520380000000003</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="61.5">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>9</v>
@@ -1510,20 +1618,20 @@
         <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="J10" s="1">
         <v>39.114306587107599</v>
@@ -1532,16 +1640,16 @@
         <v>-77.539617175199197</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="61.5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="43" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A10+1</f>
         <v>10</v>
@@ -1559,16 +1667,16 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>87</v>
+        <v>56</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J11" s="1">
         <v>39.114306587107599</v>
@@ -1577,16 +1685,16 @@
         <v>-77.539617175199197</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="61.5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1604,16 +1712,16 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J12" s="1">
         <v>38.917318174769903</v>
@@ -1622,16 +1730,16 @@
         <v>-77.231870559863694</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="61.5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f>A12+1</f>
         <v>12</v>
@@ -1643,7 +1751,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -1652,7 +1760,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1660,7 +1768,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="102.5">
+    <row r="14" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1672,7 +1780,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
@@ -1681,7 +1789,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1689,7 +1797,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="41">
+    <row r="15" spans="1:14" ht="38" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1707,13 +1815,13 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>26</v>
@@ -1725,16 +1833,16 @@
         <v>-77.555404002188297</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="61.5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1752,16 +1860,16 @@
         <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="J16" s="1">
         <v>37.610656959136698</v>
@@ -1770,16 +1878,16 @@
         <v>-77.340073015724201</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="M16" s="5" t="s">
         <v>145</v>
       </c>
+      <c r="M16" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="N16" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="82">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1797,16 +1905,16 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="J17" s="1">
         <v>39.114571664302197</v>
@@ -1815,16 +1923,16 @@
         <v>-77.5405475733521</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="61.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1833,25 +1941,25 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="J18" s="1">
         <v>0</v>
@@ -1860,16 +1968,16 @@
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="61.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="124" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1878,25 +1986,25 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
@@ -1905,16 +2013,16 @@
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="82">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1923,25 +2031,25 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
@@ -1950,16 +2058,16 @@
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="61.5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1968,25 +2076,25 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1995,16 +2103,16 @@
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="82">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2013,25 +2121,25 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
@@ -2040,16 +2148,16 @@
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="123">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2058,25 +2166,25 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
@@ -2085,41 +2193,41 @@
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="123">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J24" s="1">
         <v>40.439188049657297</v>
@@ -2128,43 +2236,43 @@
         <v>-80.001456359819201</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>150</v>
+        <v>163</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="143.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J25" s="1">
         <v>40.437306095099501</v>
@@ -2173,43 +2281,43 @@
         <v>-80.001021344478104</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="102.5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="J26" s="1">
         <v>40.349269889276798</v>
@@ -2218,43 +2326,43 @@
         <v>-79.832162824794494</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>151</v>
+        <v>164</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="82">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="43" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J27" s="1">
         <v>40.4391327899964</v>
@@ -2263,86 +2371,86 @@
         <v>-79.994721902148598</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M27" s="7" t="s">
-        <v>152</v>
+        <v>163</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="102.5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>153</v>
+        <v>165</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="82">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="43" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J29" s="1">
         <v>40.4006205568135</v>
@@ -2351,43 +2459,43 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M29" s="10" t="s">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="82">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="43" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J30" s="1">
         <v>40.4006205568135</v>
@@ -2396,40 +2504,40 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="102.5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="43" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1">
@@ -2439,255 +2547,728 @@
         <v>-79.835243102149704</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="184.5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="I32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>167</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="225.5">
+      <c r="N32" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I33" s="13" t="s">
+      <c r="H33" s="1" t="s">
         <v>171</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" ht="205">
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F34" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14" t="s">
-        <v>173</v>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="N34" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="14"/>
+        <v>175</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="123">
+      <c r="N35" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D36" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="14"/>
+      <c r="D36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="123">
+      <c r="N36" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f>A32+1</f>
         <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="14" t="s">
-        <v>177</v>
+      <c r="F37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="123">
+      <c r="N37" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" t="s">
-        <v>183</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>179</v>
+      <c r="F38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="N38" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="123">
+      <c r="N38" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>181</v>
+        <v>175</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" t="s">
-        <v>183</v>
+      <c r="F39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="L40" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="57" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="J40" s="2">
+        <v>38.906303508879397</v>
+      </c>
+      <c r="K40" s="2">
+        <v>-77.222641329237604</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J41" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="K41" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J42" s="2">
+        <v>38.875816034503501</v>
+      </c>
+      <c r="K42" s="2">
+        <v>-77.435718373358995</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J43" s="2">
+        <v>38.873610192974397</v>
+      </c>
+      <c r="K43" s="2">
+        <v>-77.3055466310296</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="J44" s="2">
+        <v>38.868590773014198</v>
+      </c>
+      <c r="K44" s="2">
+        <v>-77.224144877053305</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="147" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J45" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="K45" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J46" s="2">
+        <v>38.8060490968736</v>
+      </c>
+      <c r="K46" s="2">
+        <v>-77.181676502196197</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J47" s="2">
+        <v>38.8553917225858</v>
+      </c>
+      <c r="K47" s="2">
+        <v>-77.362718702194798</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J48" s="2">
+        <v>38.854251580169802</v>
+      </c>
+      <c r="K48" s="2">
+        <v>-77.356579302194902</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="E54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added in information on the Rmd and excel sheet
</commit_message>
<xml_diff>
--- a/Qualitative_research/Research-Foster_care-New_col_added.xlsx
+++ b/Qualitative_research/Research-Foster_care-New_col_added.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaidarobinson/Desktop/dspg/2021_DSPG_Loudoun/Qualitative_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E369416-64D5-954C-9143-0B19F25A5BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34966F91-5E99-A94F-BF62-2DB649DEA382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
+    <workbookView xWindow="2720" yWindow="2760" windowWidth="28800" windowHeight="16440" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="242">
   <si>
     <t>ID</t>
   </si>
@@ -732,6 +732,51 @@
   </si>
   <si>
     <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/tops</t>
+  </si>
+  <si>
+    <t>TIP- Transition to Independence Program</t>
+  </si>
+  <si>
+    <t>Must be enrolled at the Davis and Pulley Career Centers and have an IEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This programs helps those students with IEP build employable skills at the local community colleges. It helps them have work-based learning, coordinate to postsecondary resources and services, provide an opportunity to experience post-secondary education and help them achieve their goals. </t>
+  </si>
+  <si>
+    <t>https://www.fcps.edu/academics/academic-overview/special-education-instruction/career-and-transition-services/transition-to-independence</t>
+  </si>
+  <si>
+    <t>Taxi Access</t>
+  </si>
+  <si>
+    <t>Must be a resident of fairfax county or the City of Fairfax. Must be a registered user of Metro Access.</t>
+  </si>
+  <si>
+    <t>https://www.fairfaxcounty.gov/neighborhood-community-services/transportation/taxi-voucherprogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This program allows qualified users to travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 8 coupon books per year (July 1- June 30)</t>
+  </si>
+  <si>
+    <t>Department of Neighborhood and Community Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This program allows qualified users to travel affordable, safely, and independently with the purchase of a discounted taxicab coupon. Cost $10 per $33 coupon book. 16 coupon books per year (July 1- June 30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must be a resident of Fairfax County or the City of Fairfax. Annual income must be 225% below Federal Poverty Guidelines. </t>
+  </si>
+  <si>
+    <t>Dial-A_Ride</t>
+  </si>
+  <si>
+    <t>Fairfax County Travel Training</t>
+  </si>
+  <si>
+    <t>Must be a resident of Fairfax county or the City of Fairfax.</t>
+  </si>
+  <si>
+    <t>This program is designed for independent senior services, but it is open for student travelers  who want to learn about the public transit system. This  course is designed to help citizens plan their trip, read bus and rail schedules, pay bus fares, transfer, reach specific destination, access local transportation resources. Call the Travel Training program at 703-877-5800</t>
   </si>
 </sst>
 </file>
@@ -832,7 +877,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -864,6 +909,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1181,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A48" sqref="A40:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="M39" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1383,7 +1431,7 @@
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A53" si="0">A4+1</f>
+        <f t="shared" ref="A5:A54" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3032,51 +3080,43 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="147" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="63" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>213</v>
+        <v>17</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>218</v>
+        <v>50</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J45" s="2">
-        <v>38.8060490968736</v>
-      </c>
-      <c r="K45" s="2">
-        <v>-77.181676502196197</v>
+        <v>229</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="N45" s="13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="147" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -3094,14 +3134,14 @@
       <c r="F46" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="G46" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>217</v>
+      <c r="I46" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="J46" s="2">
         <v>38.8060490968736</v>
@@ -3128,7 +3168,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>8</v>
@@ -3137,28 +3177,28 @@
         <v>49</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>218</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J47" s="2">
-        <v>38.8553917225858</v>
+        <v>38.8060490968736</v>
       </c>
       <c r="K47" s="2">
-        <v>-77.362718702194798</v>
+        <v>-77.181676502196197</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="168" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3167,40 +3207,40 @@
         <v>189</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>221</v>
       </c>
       <c r="J48" s="2">
-        <v>38.854251580169802</v>
+        <v>38.8553917225858</v>
       </c>
       <c r="K48" s="2">
-        <v>-77.356579302194902</v>
+        <v>-77.362718702194798</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>189</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="168" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3208,11 +3248,41 @@
       <c r="B49" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="C49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J49" s="2">
+        <v>38.854251580169802</v>
+      </c>
+      <c r="K49" s="2">
+        <v>-77.356579302194902</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3220,11 +3290,38 @@
       <c r="B50" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="C50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N50" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3232,11 +3329,38 @@
       <c r="B51" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="C51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="84" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3244,11 +3368,36 @@
       <c r="B52" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="C52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="F52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3260,13 +3409,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="E56" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3276,8 +3437,11 @@
     <hyperlink ref="N34" r:id="rId2" xr:uid="{A4D4722A-F053-934D-97DC-12F1F10D2CC7}"/>
     <hyperlink ref="N36" r:id="rId3" xr:uid="{6B18FC7C-EE3D-6D44-B9DF-7F93B7653470}"/>
     <hyperlink ref="N37:N38" r:id="rId4" display="https://www.alleghenycounty.us/Human-Services/Programs-Services/Basic-Needs/Health-Insurance.aspx" xr:uid="{A6720D7E-3399-D843-87D0-0CB86745C76A}"/>
+    <hyperlink ref="N50" r:id="rId5" xr:uid="{93C7EECE-AB5B-EC4C-A9D6-5929F9D968B8}"/>
+    <hyperlink ref="N51" r:id="rId6" xr:uid="{C862D923-15DC-374D-B1CA-DF6D3EA8A530}"/>
+    <hyperlink ref="N45" r:id="rId7" xr:uid="{7BB821AF-4CAD-9741-8FA6-C0B727864735}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>